<commit_message>
Update timeline of draft WBS
</commit_message>
<xml_diff>
--- a/WBS Draft.xlsx
+++ b/WBS Draft.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2b21d9556be71756/Griffith/2810ICT Software Technologies/Assignment/2810ICT-2022-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="257" documentId="8_{97E3422E-7BAE-44B5-A3D1-192CBEFB2816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39B7899E-7D8D-4E6B-8E3F-F3F6AE112F4F}"/>
+  <xr:revisionPtr revIDLastSave="299" documentId="8_{97E3422E-7BAE-44B5-A3D1-192CBEFB2816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8ECC2F60-1B5C-43C0-BA79-A983F483A4B7}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22560" windowHeight="14440" xr2:uid="{6CBAA0E4-AAB6-4A55-8BA7-A93F0BFF7F34}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="22560" windowHeight="14440" xr2:uid="{6CBAA0E4-AAB6-4A55-8BA7-A93F0BFF7F34}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -229,7 +229,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,8 +254,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -412,11 +418,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -426,7 +458,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -452,6 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -485,10 +517,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -806,14 +859,14 @@
   <dimension ref="A1:AF112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="M35" sqref="M35"/>
+      <selection activeCell="AB54" sqref="AB54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="110" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:32" x14ac:dyDescent="0.35">
@@ -947,11 +1000,11 @@
       </c>
     </row>
     <row r="3" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -959,9 +1012,30 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
     </row>
     <row r="4" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
@@ -973,9 +1047,30 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
     </row>
     <row r="5" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="29" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2"/>
@@ -987,11 +1082,33 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
     </row>
     <row r="6" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="29" t="s">
         <v>4</v>
       </c>
+      <c r="C6" s="1"/>
       <c r="D6" s="2"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1000,27 +1117,69 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
     </row>
     <row r="7" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="30" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
     </row>
     <row r="8" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="29" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1"/>
-      <c r="D8" s="28"/>
+      <c r="D8" s="16"/>
       <c r="E8" s="2"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1028,443 +1187,1115 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
     </row>
     <row r="9" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="29" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
       <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
     </row>
     <row r="10" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="29" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
       <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
     </row>
     <row r="11" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="29" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
       <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
     </row>
     <row r="12" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="29" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
       <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
     </row>
     <row r="13" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
+      <c r="J13" s="36"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="36"/>
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
     </row>
     <row r="14" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
     </row>
     <row r="15" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
       <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="1"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
     </row>
     <row r="16" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
       <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B17" s="4" t="s">
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+    </row>
+    <row r="17" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B17" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
       <c r="K17" s="1"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B18" s="4" t="s">
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+    </row>
+    <row r="18" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B18" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
       <c r="K18" s="1"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B19" s="4" t="s">
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+    </row>
+    <row r="19" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B19" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
       <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B20" s="4" t="s">
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+    </row>
+    <row r="20" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B20" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
       <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B21" s="4" t="s">
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+    </row>
+    <row r="21" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B21" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B22" s="4" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+    </row>
+    <row r="22" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B22" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
       <c r="K22" s="1"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B23" s="4" t="s">
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+    </row>
+    <row r="23" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B23" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
       <c r="K23" s="1"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B24" s="4" t="s">
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+    </row>
+    <row r="24" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B24" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
       <c r="K24" s="1"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B25" s="4" t="s">
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+    </row>
+    <row r="25" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B25" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
       <c r="K25" s="1"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B26" s="9" t="s">
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+    </row>
+    <row r="26" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B26" s="33" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B27" s="6" t="s">
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
+      <c r="P26" s="36"/>
+      <c r="Q26" s="36"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="36"/>
+      <c r="T26" s="36"/>
+      <c r="U26" s="36"/>
+      <c r="V26" s="36"/>
+      <c r="W26" s="36"/>
+      <c r="X26" s="36"/>
+      <c r="Y26" s="36"/>
+      <c r="Z26" s="36"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="1"/>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
+    </row>
+    <row r="27" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B27" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="16"/>
       <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B28" s="3" t="s">
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+    </row>
+    <row r="28" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B28" s="29" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B29" s="3" t="s">
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
+      <c r="U28" s="2"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+    </row>
+    <row r="29" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B29" s="29" t="s">
         <v>27</v>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B30" s="3" t="s">
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="16"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="2"/>
+      <c r="S29" s="2"/>
+      <c r="T29" s="2"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="2"/>
+      <c r="X29" s="2"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="1"/>
+    </row>
+    <row r="30" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B30" s="29" t="s">
         <v>28</v>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B31" s="3" t="s">
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="2"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="1"/>
+      <c r="AF30" s="1"/>
+    </row>
+    <row r="31" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B31" s="29" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B32" s="3" t="s">
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2"/>
+      <c r="Q31" s="2"/>
+      <c r="R31" s="2"/>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="2"/>
+      <c r="X31" s="2"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+      <c r="AF31" s="1"/>
+    </row>
+    <row r="32" spans="2:32" x14ac:dyDescent="0.35">
+      <c r="B32" s="29" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2"/>
+      <c r="Q32" s="2"/>
+      <c r="R32" s="2"/>
+      <c r="S32" s="2"/>
+      <c r="T32" s="2"/>
+      <c r="U32" s="2"/>
+      <c r="V32" s="2"/>
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="1"/>
+      <c r="AF32" s="1"/>
     </row>
     <row r="33" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="29" t="s">
         <v>31</v>
       </c>
       <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2"/>
+      <c r="Q33" s="2"/>
+      <c r="R33" s="2"/>
+      <c r="S33" s="2"/>
+      <c r="T33" s="2"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="2"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="1"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="1"/>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="1"/>
+      <c r="AF33" s="1"/>
     </row>
     <row r="34" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B34" s="29" t="s">
+      <c r="B34" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="1"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="16"/>
       <c r="K34" s="1"/>
+      <c r="L34" s="36"/>
+      <c r="M34" s="36"/>
+      <c r="N34" s="36"/>
+      <c r="O34" s="36"/>
+      <c r="P34" s="36"/>
+      <c r="Q34" s="36"/>
+      <c r="R34" s="36"/>
+      <c r="S34" s="36"/>
+      <c r="T34" s="36"/>
+      <c r="U34" s="36"/>
+      <c r="V34" s="36"/>
+      <c r="W34" s="36"/>
+      <c r="X34" s="36"/>
+      <c r="Y34" s="36"/>
+      <c r="Z34" s="36"/>
+      <c r="AA34" s="1"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="1"/>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="1"/>
+      <c r="AF34" s="1"/>
     </row>
     <row r="35" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="29" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="1"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="16"/>
       <c r="K35" s="1"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="2"/>
+      <c r="AA35" s="1"/>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="1"/>
+      <c r="AD35" s="1"/>
+      <c r="AE35" s="1"/>
+      <c r="AF35" s="1"/>
     </row>
     <row r="36" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="29" t="s">
         <v>34</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="1"/>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="16"/>
+      <c r="H36" s="16"/>
+      <c r="I36" s="16"/>
+      <c r="J36" s="16"/>
       <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="2"/>
+      <c r="AB36" s="2"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="1"/>
+      <c r="AF36" s="1"/>
     </row>
     <row r="37" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="1"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="16"/>
+      <c r="I37" s="16"/>
+      <c r="J37" s="16"/>
       <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="2"/>
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="1"/>
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="1"/>
+      <c r="AF37" s="1"/>
     </row>
     <row r="38" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="29" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="1"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
+      <c r="H38" s="16"/>
+      <c r="I38" s="16"/>
+      <c r="J38" s="16"/>
       <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+      <c r="Z38" s="1"/>
+      <c r="AA38" s="1"/>
+      <c r="AB38" s="1"/>
+      <c r="AC38" s="2"/>
+      <c r="AD38" s="2"/>
+      <c r="AE38" s="1"/>
+      <c r="AF38" s="1"/>
     </row>
     <row r="39" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
+      <c r="C39" s="36"/>
+      <c r="D39" s="36"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="36"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="36"/>
+      <c r="M39" s="36"/>
+      <c r="N39" s="36"/>
+      <c r="O39" s="36"/>
+      <c r="P39" s="36"/>
+      <c r="Q39" s="36"/>
+      <c r="R39" s="36"/>
+      <c r="S39" s="36"/>
+      <c r="T39" s="36"/>
+      <c r="U39" s="36"/>
+      <c r="V39" s="36"/>
+      <c r="W39" s="36"/>
+      <c r="X39" s="36"/>
+      <c r="Y39" s="36"/>
+      <c r="Z39" s="36"/>
+      <c r="AA39" s="36"/>
+      <c r="AB39" s="36"/>
+      <c r="AC39" s="36"/>
+      <c r="AD39" s="36"/>
+      <c r="AE39" s="1"/>
+      <c r="AF39" s="1"/>
     </row>
     <row r="40" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="29" t="s">
         <v>38</v>
       </c>
       <c r="C40" s="2"/>
@@ -1495,9 +2326,11 @@
       <c r="AB40" s="2"/>
       <c r="AC40" s="2"/>
       <c r="AD40" s="2"/>
+      <c r="AE40" s="1"/>
+      <c r="AF40" s="1"/>
     </row>
     <row r="41" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="29" t="s">
         <v>39</v>
       </c>
       <c r="C41" s="2"/>
@@ -1528,9 +2361,11 @@
       <c r="AB41" s="2"/>
       <c r="AC41" s="2"/>
       <c r="AD41" s="2"/>
+      <c r="AE41" s="1"/>
+      <c r="AF41" s="1"/>
     </row>
     <row r="42" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="30" t="s">
         <v>40</v>
       </c>
       <c r="C42" s="1"/>
@@ -1542,9 +2377,30 @@
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1"/>
+      <c r="S42" s="1"/>
+      <c r="T42" s="1"/>
+      <c r="U42" s="1"/>
+      <c r="V42" s="1"/>
+      <c r="W42" s="1"/>
+      <c r="X42" s="1"/>
+      <c r="Y42" s="1"/>
+      <c r="Z42" s="1"/>
+      <c r="AA42" s="1"/>
+      <c r="AB42" s="1"/>
+      <c r="AC42" s="1"/>
+      <c r="AD42" s="1"/>
+      <c r="AE42" s="36"/>
+      <c r="AF42" s="36"/>
     </row>
     <row r="43" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="29" t="s">
         <v>41</v>
       </c>
       <c r="C43" s="1"/>
@@ -1554,11 +2410,32 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1"/>
+      <c r="S43" s="1"/>
+      <c r="T43" s="1"/>
+      <c r="U43" s="1"/>
+      <c r="V43" s="1"/>
+      <c r="W43" s="1"/>
+      <c r="X43" s="1"/>
+      <c r="Y43" s="1"/>
+      <c r="Z43" s="1"/>
+      <c r="AA43" s="1"/>
+      <c r="AB43" s="1"/>
+      <c r="AC43" s="1"/>
+      <c r="AD43" s="1"/>
       <c r="AE43" s="2"/>
       <c r="AF43" s="2"/>
     </row>
     <row r="44" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="29" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="1"/>
@@ -1568,13 +2445,64 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1"/>
+      <c r="AA44" s="1"/>
+      <c r="AB44" s="1"/>
+      <c r="AC44" s="1"/>
+      <c r="AD44" s="1"/>
       <c r="AE44" s="2"/>
       <c r="AF44" s="2"/>
     </row>
     <row r="45" spans="2:32" x14ac:dyDescent="0.35">
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1"/>
+      <c r="S45" s="1"/>
+      <c r="T45" s="1"/>
+      <c r="U45" s="1"/>
+      <c r="V45" s="1"/>
+      <c r="W45" s="1"/>
+      <c r="X45" s="1"/>
+      <c r="Y45" s="1"/>
+      <c r="Z45" s="1"/>
+      <c r="AA45" s="1"/>
+      <c r="AB45" s="1"/>
+      <c r="AC45" s="1"/>
+      <c r="AD45" s="1"/>
+      <c r="AE45" s="1"/>
+      <c r="AF45" s="2"/>
     </row>
     <row r="51" spans="2:11" ht="8.15" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="52" spans="2:11" ht="29.15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1625,394 +2553,394 @@
         <v>48</v>
       </c>
       <c r="B65" s="18"/>
-      <c r="C65" s="11" t="s">
+      <c r="C65" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D65" s="11" t="s">
+      <c r="D65" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E65" s="11" t="s">
+      <c r="E65" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="11"/>
+      <c r="F65" s="10"/>
+      <c r="G65" s="10"/>
+      <c r="H65" s="10"/>
+      <c r="I65" s="10"/>
+      <c r="J65" s="10"/>
+      <c r="K65" s="10"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A66" s="14">
+      <c r="A66" s="13">
         <v>1</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C66" s="11"/>
-      <c r="D66" s="11"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="11"/>
-      <c r="K66" s="11"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="10"/>
+      <c r="F66" s="10"/>
+      <c r="G66" s="10"/>
+      <c r="H66" s="10"/>
+      <c r="I66" s="10"/>
+      <c r="J66" s="10"/>
+      <c r="K66" s="10"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A67" s="14">
+      <c r="A67" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="11"/>
-      <c r="K67" s="11"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="F67" s="10"/>
+      <c r="G67" s="10"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="10"/>
+      <c r="J67" s="10"/>
+      <c r="K67" s="10"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A68" s="14">
+      <c r="A68" s="13">
         <v>1.2</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C68" s="11"/>
-      <c r="D68" s="11"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="11"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
+      <c r="E68" s="10"/>
+      <c r="F68" s="10"/>
+      <c r="G68" s="10"/>
+      <c r="H68" s="10"/>
+      <c r="I68" s="10"/>
+      <c r="J68" s="10"/>
+      <c r="K68" s="10"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A69" s="14">
+      <c r="A69" s="13">
         <v>1.3</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="11"/>
-      <c r="D69" s="11"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
-      <c r="K69" s="11"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="10"/>
+      <c r="I69" s="10"/>
+      <c r="J69" s="10"/>
+      <c r="K69" s="10"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A70" s="14">
+      <c r="A70" s="13">
         <v>2</v>
       </c>
-      <c r="B70" s="7" t="s">
+      <c r="B70" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C70" s="11"/>
-      <c r="D70" s="11"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="10"/>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10"/>
+      <c r="J70" s="10"/>
+      <c r="K70" s="10"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A71" s="14">
+      <c r="A71" s="13">
         <v>2.1</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C71" s="11"/>
-      <c r="D71" s="11"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
-      <c r="I71" s="11"/>
-      <c r="J71" s="11"/>
-      <c r="K71" s="11"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="10"/>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10"/>
+      <c r="J71" s="10"/>
+      <c r="K71" s="10"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A72" s="14">
+      <c r="A72" s="13">
         <v>2.2000000000000002</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
-      <c r="I72" s="11"/>
-      <c r="J72" s="11"/>
-      <c r="K72" s="11"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="10"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A73" s="14">
+      <c r="A73" s="13">
         <v>2.2999999999999998</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="11"/>
-      <c r="J73" s="11"/>
-      <c r="K73" s="11"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
+      <c r="F73" s="10"/>
+      <c r="G73" s="10"/>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10"/>
+      <c r="K73" s="10"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A74" s="14">
+      <c r="A74" s="13">
         <v>2.4</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="11"/>
-      <c r="K74" s="11"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10"/>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10"/>
+      <c r="H74" s="10"/>
+      <c r="I74" s="10"/>
+      <c r="J74" s="10"/>
+      <c r="K74" s="10"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A75" s="14">
+      <c r="A75" s="13">
         <v>2.5</v>
       </c>
       <c r="B75" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C75" s="11"/>
-      <c r="D75" s="11"/>
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
-      <c r="I75" s="11"/>
-      <c r="J75" s="11"/>
-      <c r="K75" s="11"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
+      <c r="K75" s="10"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A76" s="14">
+      <c r="A76" s="13">
         <v>3</v>
       </c>
-      <c r="B76" s="15" t="s">
+      <c r="B76" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="11"/>
-      <c r="J76" s="11"/>
-      <c r="K76" s="11"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10"/>
+      <c r="J76" s="10"/>
+      <c r="K76" s="10"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A77" s="14">
+      <c r="A77" s="13">
         <v>3.1</v>
       </c>
       <c r="B77" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C77" s="12"/>
-      <c r="D77" s="11"/>
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="11"/>
-      <c r="K77" s="11"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+      <c r="J77" s="10"/>
+      <c r="K77" s="10"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A78" s="14">
+      <c r="A78" s="13">
         <v>3.2</v>
       </c>
       <c r="B78" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C78" s="12"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
-      <c r="I78" s="11"/>
-      <c r="J78" s="11"/>
-      <c r="K78" s="11"/>
+      <c r="C78" s="11"/>
+      <c r="D78" s="10"/>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+      <c r="J78" s="10"/>
+      <c r="K78" s="10"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A79" s="14">
+      <c r="A79" s="13">
         <v>3.3</v>
       </c>
       <c r="B79" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C79" s="12"/>
-      <c r="D79" s="11"/>
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="11"/>
-      <c r="K79" s="11"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="10"/>
+      <c r="E79" s="10"/>
+      <c r="F79" s="10"/>
+      <c r="G79" s="10"/>
+      <c r="H79" s="10"/>
+      <c r="I79" s="10"/>
+      <c r="J79" s="10"/>
+      <c r="K79" s="10"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A80" s="14">
+      <c r="A80" s="13">
         <v>3.4</v>
       </c>
       <c r="B80" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C80" s="12"/>
-      <c r="D80" s="11"/>
-      <c r="E80" s="11"/>
-      <c r="F80" s="11"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11"/>
-      <c r="I80" s="11"/>
-      <c r="J80" s="11"/>
-      <c r="K80" s="11"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="10"/>
+      <c r="E80" s="10"/>
+      <c r="F80" s="10"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="10"/>
+      <c r="I80" s="10"/>
+      <c r="J80" s="10"/>
+      <c r="K80" s="10"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A81" s="14">
+      <c r="A81" s="13">
         <v>3.5</v>
       </c>
       <c r="B81" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C81" s="12"/>
-      <c r="D81" s="11"/>
-      <c r="E81" s="11"/>
-      <c r="F81" s="11"/>
-      <c r="G81" s="11"/>
-      <c r="H81" s="11"/>
-      <c r="I81" s="11"/>
-      <c r="J81" s="11"/>
-      <c r="K81" s="11"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="10"/>
+      <c r="E81" s="10"/>
+      <c r="F81" s="10"/>
+      <c r="G81" s="10"/>
+      <c r="H81" s="10"/>
+      <c r="I81" s="10"/>
+      <c r="J81" s="10"/>
+      <c r="K81" s="10"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A82" s="14">
+      <c r="A82" s="13">
         <v>3.6</v>
       </c>
       <c r="B82" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C82" s="12"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
-      <c r="I82" s="11"/>
-      <c r="J82" s="11"/>
-      <c r="K82" s="11"/>
+      <c r="C82" s="11"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="10"/>
+      <c r="F82" s="10"/>
+      <c r="G82" s="10"/>
+      <c r="H82" s="10"/>
+      <c r="I82" s="10"/>
+      <c r="J82" s="10"/>
+      <c r="K82" s="10"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A83" s="14">
+      <c r="A83" s="13">
         <v>3.7</v>
       </c>
       <c r="B83" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C83" s="12"/>
-      <c r="D83" s="11"/>
-      <c r="E83" s="11"/>
-      <c r="F83" s="11"/>
-      <c r="G83" s="11"/>
-      <c r="H83" s="11"/>
-      <c r="I83" s="11"/>
-      <c r="J83" s="11"/>
-      <c r="K83" s="11"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="10"/>
+      <c r="E83" s="10"/>
+      <c r="F83" s="10"/>
+      <c r="G83" s="10"/>
+      <c r="H83" s="10"/>
+      <c r="I83" s="10"/>
+      <c r="J83" s="10"/>
+      <c r="K83" s="10"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A84" s="14">
+      <c r="A84" s="13">
         <v>3.8</v>
       </c>
       <c r="B84" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C84" s="12"/>
-      <c r="D84" s="11"/>
-      <c r="E84" s="11"/>
-      <c r="F84" s="11"/>
-      <c r="G84" s="11"/>
-      <c r="H84" s="11"/>
-      <c r="I84" s="11"/>
-      <c r="J84" s="11"/>
-      <c r="K84" s="11"/>
+      <c r="C84" s="11"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="10"/>
+      <c r="F84" s="10"/>
+      <c r="G84" s="10"/>
+      <c r="H84" s="10"/>
+      <c r="I84" s="10"/>
+      <c r="J84" s="10"/>
+      <c r="K84" s="10"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A85" s="14">
+      <c r="A85" s="13">
         <v>3.9</v>
       </c>
       <c r="B85" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C85" s="12"/>
-      <c r="D85" s="11"/>
-      <c r="E85" s="11"/>
-      <c r="F85" s="11"/>
-      <c r="G85" s="11"/>
-      <c r="H85" s="11"/>
-      <c r="I85" s="11"/>
-      <c r="J85" s="11"/>
-      <c r="K85" s="11"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="10"/>
+      <c r="E85" s="10"/>
+      <c r="F85" s="10"/>
+      <c r="G85" s="10"/>
+      <c r="H85" s="10"/>
+      <c r="I85" s="10"/>
+      <c r="J85" s="10"/>
+      <c r="K85" s="10"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A86" s="13">
+      <c r="A86" s="12">
         <v>3.1</v>
       </c>
       <c r="B86" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C86" s="12"/>
-      <c r="D86" s="11"/>
-      <c r="E86" s="11"/>
-      <c r="F86" s="11"/>
-      <c r="G86" s="11"/>
-      <c r="H86" s="11"/>
-      <c r="I86" s="11"/>
-      <c r="J86" s="11"/>
-      <c r="K86" s="11"/>
+      <c r="C86" s="11"/>
+      <c r="D86" s="10"/>
+      <c r="E86" s="10"/>
+      <c r="F86" s="10"/>
+      <c r="G86" s="10"/>
+      <c r="H86" s="10"/>
+      <c r="I86" s="10"/>
+      <c r="J86" s="10"/>
+      <c r="K86" s="10"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A87" s="13">
+      <c r="A87" s="12">
         <v>3.11</v>
       </c>
       <c r="B87" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C87" s="12"/>
-      <c r="D87" s="11"/>
-      <c r="E87" s="11"/>
-      <c r="F87" s="11"/>
-      <c r="G87" s="11"/>
-      <c r="H87" s="11"/>
-      <c r="I87" s="11"/>
-      <c r="J87" s="11"/>
-      <c r="K87" s="11"/>
+      <c r="C87" s="11"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
+      <c r="F87" s="10"/>
+      <c r="G87" s="10"/>
+      <c r="H87" s="10"/>
+      <c r="I87" s="10"/>
+      <c r="J87" s="10"/>
+      <c r="K87" s="10"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88">
@@ -2021,321 +2949,321 @@
       <c r="B88" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C88" s="12"/>
-      <c r="D88" s="11"/>
-      <c r="E88" s="11"/>
-      <c r="F88" s="11"/>
-      <c r="G88" s="11"/>
-      <c r="H88" s="11"/>
-      <c r="I88" s="11"/>
-      <c r="J88" s="11"/>
-      <c r="K88" s="11"/>
+      <c r="C88" s="11"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="10"/>
+      <c r="F88" s="10"/>
+      <c r="G88" s="10"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="10"/>
+      <c r="J88" s="10"/>
+      <c r="K88" s="10"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A89" s="14">
+      <c r="A89" s="13">
         <v>4</v>
       </c>
-      <c r="B89" s="9" t="s">
+      <c r="B89" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C89" s="11"/>
-      <c r="D89" s="11"/>
-      <c r="E89" s="11"/>
-      <c r="F89" s="11"/>
-      <c r="G89" s="11"/>
-      <c r="H89" s="11"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="11"/>
-      <c r="K89" s="11"/>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="10"/>
+      <c r="F89" s="10"/>
+      <c r="G89" s="10"/>
+      <c r="H89" s="10"/>
+      <c r="I89" s="10"/>
+      <c r="J89" s="10"/>
+      <c r="K89" s="10"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A90" s="14">
+      <c r="A90" s="13">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B90" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C90" s="11"/>
-      <c r="D90" s="11"/>
-      <c r="E90" s="11"/>
-      <c r="F90" s="11"/>
-      <c r="G90" s="11"/>
-      <c r="H90" s="11"/>
-      <c r="I90" s="11"/>
-      <c r="J90" s="11"/>
-      <c r="K90" s="11"/>
+      <c r="C90" s="10"/>
+      <c r="D90" s="10"/>
+      <c r="E90" s="10"/>
+      <c r="F90" s="10"/>
+      <c r="G90" s="10"/>
+      <c r="H90" s="10"/>
+      <c r="I90" s="10"/>
+      <c r="J90" s="10"/>
+      <c r="K90" s="10"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A91" s="14">
+      <c r="A91" s="13">
         <v>4.2</v>
       </c>
       <c r="B91" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
-      <c r="G91" s="11"/>
-      <c r="H91" s="11"/>
-      <c r="I91" s="11"/>
-      <c r="J91" s="11"/>
-      <c r="K91" s="11"/>
+      <c r="C91" s="10"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="10"/>
+      <c r="F91" s="10"/>
+      <c r="G91" s="10"/>
+      <c r="H91" s="10"/>
+      <c r="I91" s="10"/>
+      <c r="J91" s="10"/>
+      <c r="K91" s="10"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A92" s="14">
+      <c r="A92" s="13">
         <v>4.3</v>
       </c>
       <c r="B92" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C92" s="11"/>
-      <c r="D92" s="11"/>
-      <c r="E92" s="11"/>
-      <c r="F92" s="11"/>
-      <c r="G92" s="11"/>
-      <c r="H92" s="11"/>
-      <c r="I92" s="11"/>
-      <c r="J92" s="11"/>
-      <c r="K92" s="11"/>
+      <c r="C92" s="10"/>
+      <c r="D92" s="10"/>
+      <c r="E92" s="10"/>
+      <c r="F92" s="10"/>
+      <c r="G92" s="10"/>
+      <c r="H92" s="10"/>
+      <c r="I92" s="10"/>
+      <c r="J92" s="10"/>
+      <c r="K92" s="10"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A93" s="14">
+      <c r="A93" s="13">
         <v>4.4000000000000004</v>
       </c>
       <c r="B93" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C93" s="11"/>
-      <c r="D93" s="11"/>
-      <c r="E93" s="11"/>
-      <c r="F93" s="11"/>
-      <c r="G93" s="11"/>
-      <c r="H93" s="11"/>
-      <c r="I93" s="11"/>
-      <c r="J93" s="11"/>
-      <c r="K93" s="11"/>
+      <c r="C93" s="10"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="10"/>
+      <c r="F93" s="10"/>
+      <c r="G93" s="10"/>
+      <c r="H93" s="10"/>
+      <c r="I93" s="10"/>
+      <c r="J93" s="10"/>
+      <c r="K93" s="10"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A94" s="14">
+      <c r="A94" s="13">
         <v>4.5</v>
       </c>
       <c r="B94" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
-      <c r="E94" s="11"/>
-      <c r="F94" s="11"/>
-      <c r="G94" s="11"/>
-      <c r="H94" s="11"/>
-      <c r="I94" s="11"/>
-      <c r="J94" s="11"/>
-      <c r="K94" s="11"/>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="10"/>
+      <c r="F94" s="10"/>
+      <c r="G94" s="10"/>
+      <c r="H94" s="10"/>
+      <c r="I94" s="10"/>
+      <c r="J94" s="10"/>
+      <c r="K94" s="10"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A95" s="14">
+      <c r="A95" s="13">
         <v>4.5999999999999996</v>
       </c>
       <c r="B95" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
-      <c r="E95" s="11"/>
-      <c r="F95" s="11"/>
-      <c r="G95" s="11"/>
-      <c r="H95" s="11"/>
-      <c r="I95" s="11"/>
-      <c r="J95" s="11"/>
-      <c r="K95" s="11"/>
+      <c r="C95" s="10"/>
+      <c r="D95" s="10"/>
+      <c r="E95" s="10"/>
+      <c r="F95" s="10"/>
+      <c r="G95" s="10"/>
+      <c r="H95" s="10"/>
+      <c r="I95" s="10"/>
+      <c r="J95" s="10"/>
+      <c r="K95" s="10"/>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A96" s="14">
+      <c r="A96" s="13">
         <v>4.7</v>
       </c>
       <c r="B96" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C96" s="11"/>
-      <c r="D96" s="11"/>
-      <c r="E96" s="11"/>
-      <c r="F96" s="11"/>
-      <c r="G96" s="11"/>
-      <c r="H96" s="11"/>
-      <c r="I96" s="11"/>
-      <c r="J96" s="11"/>
-      <c r="K96" s="11"/>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="10"/>
+      <c r="F96" s="10"/>
+      <c r="G96" s="10"/>
+      <c r="H96" s="10"/>
+      <c r="I96" s="10"/>
+      <c r="J96" s="10"/>
+      <c r="K96" s="10"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A97" s="14">
+      <c r="A97" s="13">
         <v>5</v>
       </c>
-      <c r="B97" s="7" t="s">
+      <c r="B97" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C97" s="11"/>
-      <c r="D97" s="11"/>
-      <c r="E97" s="11"/>
-      <c r="F97" s="11"/>
-      <c r="G97" s="11"/>
-      <c r="H97" s="11"/>
-      <c r="I97" s="11"/>
-      <c r="J97" s="11"/>
-      <c r="K97" s="11"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
+      <c r="F97" s="10"/>
+      <c r="G97" s="10"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="10"/>
+      <c r="J97" s="10"/>
+      <c r="K97" s="10"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A98" s="14">
+      <c r="A98" s="13">
         <v>5.0999999999999996</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C98" s="11"/>
-      <c r="D98" s="11"/>
-      <c r="E98" s="11"/>
-      <c r="F98" s="11"/>
-      <c r="G98" s="11"/>
-      <c r="H98" s="11"/>
-      <c r="I98" s="11"/>
-      <c r="J98" s="11"/>
-      <c r="K98" s="11"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
+      <c r="G98" s="10"/>
+      <c r="H98" s="10"/>
+      <c r="I98" s="10"/>
+      <c r="J98" s="10"/>
+      <c r="K98" s="10"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A99" s="14">
+      <c r="A99" s="13">
         <v>5.2</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C99" s="11"/>
-      <c r="D99" s="11"/>
-      <c r="E99" s="11"/>
-      <c r="F99" s="11"/>
-      <c r="G99" s="11"/>
-      <c r="H99" s="11"/>
-      <c r="I99" s="11"/>
-      <c r="J99" s="11"/>
-      <c r="K99" s="11"/>
+      <c r="C99" s="10"/>
+      <c r="D99" s="10"/>
+      <c r="E99" s="10"/>
+      <c r="F99" s="10"/>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="10"/>
+      <c r="J99" s="10"/>
+      <c r="K99" s="10"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A100" s="14">
+      <c r="A100" s="13">
         <v>5.3</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11"/>
-      <c r="F100" s="11"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="11"/>
-      <c r="I100" s="11"/>
-      <c r="J100" s="11"/>
-      <c r="K100" s="11"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
+      <c r="G100" s="10"/>
+      <c r="H100" s="10"/>
+      <c r="I100" s="10"/>
+      <c r="J100" s="10"/>
+      <c r="K100" s="10"/>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A101" s="14">
+      <c r="A101" s="13">
         <v>5.4</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C101" s="11"/>
-      <c r="D101" s="11"/>
-      <c r="E101" s="11"/>
-      <c r="F101" s="11"/>
-      <c r="G101" s="11"/>
-      <c r="H101" s="11"/>
-      <c r="I101" s="11"/>
-      <c r="J101" s="11"/>
-      <c r="K101" s="11"/>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
+      <c r="E101" s="10"/>
+      <c r="F101" s="10"/>
+      <c r="G101" s="10"/>
+      <c r="H101" s="10"/>
+      <c r="I101" s="10"/>
+      <c r="J101" s="10"/>
+      <c r="K101" s="10"/>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A102" s="14">
+      <c r="A102" s="13">
         <v>6</v>
       </c>
-      <c r="B102" s="7" t="s">
+      <c r="B102" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C102" s="11"/>
-      <c r="D102" s="11"/>
-      <c r="E102" s="11"/>
-      <c r="F102" s="11"/>
-      <c r="G102" s="11"/>
-      <c r="H102" s="11"/>
-      <c r="I102" s="11"/>
-      <c r="J102" s="11"/>
-      <c r="K102" s="11"/>
+      <c r="C102" s="10"/>
+      <c r="D102" s="10"/>
+      <c r="E102" s="10"/>
+      <c r="F102" s="10"/>
+      <c r="G102" s="10"/>
+      <c r="H102" s="10"/>
+      <c r="I102" s="10"/>
+      <c r="J102" s="10"/>
+      <c r="K102" s="10"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A103" s="14">
+      <c r="A103" s="13">
         <v>6.1</v>
       </c>
-      <c r="B103" s="16" t="s">
+      <c r="B103" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C103" s="11"/>
-      <c r="D103" s="11"/>
-      <c r="E103" s="11"/>
-      <c r="F103" s="11"/>
-      <c r="G103" s="11"/>
-      <c r="H103" s="11"/>
-      <c r="I103" s="11"/>
-      <c r="J103" s="11"/>
-      <c r="K103" s="11"/>
+      <c r="C103" s="10"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="10"/>
+      <c r="F103" s="10"/>
+      <c r="G103" s="10"/>
+      <c r="H103" s="10"/>
+      <c r="I103" s="10"/>
+      <c r="J103" s="10"/>
+      <c r="K103" s="10"/>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A104" s="14">
+      <c r="A104" s="13">
         <v>6.2</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C104" s="11"/>
-      <c r="D104" s="11"/>
-      <c r="E104" s="11"/>
-      <c r="F104" s="11"/>
-      <c r="G104" s="11"/>
-      <c r="H104" s="11"/>
-      <c r="I104" s="11"/>
-      <c r="J104" s="11"/>
-      <c r="K104" s="11"/>
+      <c r="C104" s="10"/>
+      <c r="D104" s="10"/>
+      <c r="E104" s="10"/>
+      <c r="F104" s="10"/>
+      <c r="G104" s="10"/>
+      <c r="H104" s="10"/>
+      <c r="I104" s="10"/>
+      <c r="J104" s="10"/>
+      <c r="K104" s="10"/>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A105" s="14">
+      <c r="A105" s="13">
         <v>7</v>
       </c>
-      <c r="B105" s="7" t="s">
+      <c r="B105" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C105" s="11"/>
-      <c r="D105" s="11"/>
-      <c r="E105" s="11"/>
-      <c r="F105" s="11"/>
-      <c r="G105" s="11"/>
-      <c r="H105" s="11"/>
-      <c r="I105" s="11"/>
-      <c r="J105" s="11"/>
-      <c r="K105" s="11"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
+      <c r="H105" s="10"/>
+      <c r="I105" s="10"/>
+      <c r="J105" s="10"/>
+      <c r="K105" s="10"/>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A106" s="14">
+      <c r="A106" s="13">
         <v>7.1</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C106" s="11"/>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="11"/>
-      <c r="G106" s="11"/>
-      <c r="H106" s="11"/>
-      <c r="I106" s="11"/>
-      <c r="J106" s="11"/>
-      <c r="K106" s="11"/>
+      <c r="C106" s="10"/>
+      <c r="D106" s="10"/>
+      <c r="E106" s="10"/>
+      <c r="F106" s="10"/>
+      <c r="G106" s="10"/>
+      <c r="H106" s="10"/>
+      <c r="I106" s="10"/>
+      <c r="J106" s="10"/>
+      <c r="K106" s="10"/>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107">
@@ -2344,35 +3272,35 @@
       <c r="B107" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C107" s="11"/>
-      <c r="D107" s="11"/>
-      <c r="E107" s="11"/>
-      <c r="F107" s="11"/>
-      <c r="G107" s="11"/>
-      <c r="H107" s="11"/>
-      <c r="I107" s="11"/>
-      <c r="J107" s="11"/>
-      <c r="K107" s="11"/>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
+      <c r="E107" s="10"/>
+      <c r="F107" s="10"/>
+      <c r="G107" s="10"/>
+      <c r="H107" s="10"/>
+      <c r="I107" s="10"/>
+      <c r="J107" s="10"/>
+      <c r="K107" s="10"/>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>7.3</v>
       </c>
-      <c r="B108" s="10" t="s">
+      <c r="B108" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A109" s="14"/>
+      <c r="A109" s="13"/>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A110" s="14"/>
+      <c r="A110" s="13"/>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A111" s="14"/>
+      <c r="A111" s="13"/>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A112" s="14"/>
+      <c r="A112" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>